<commit_message>
Fix FeatureCompatibility chart note for DxC
</commit_message>
<xml_diff>
--- a/docs/FeatureCompatibility.xlsx
+++ b/docs/FeatureCompatibility.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2592\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62A07544-A8B8-44EF-8E70-17EA0820C847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58BA46B4-6823-4DD8-8536-F21A5031EE65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38445" yWindow="435" windowWidth="28755" windowHeight="16395" xr2:uid="{46F717FF-FE5F-3D4F-A8F5-51784E44D20C}"/>
   </bookViews>
@@ -362,10 +362,10 @@
     <t>aws_tgw_directconnect</t>
   </si>
   <si>
-    <t>will forcenew</t>
-  </si>
-  <si>
     <t>directconnect_account_name</t>
+  </si>
+  <si>
+    <t>Export for this resource is not implemented yet</t>
   </si>
   <si>
     <t>dx_gateway_id</t>
@@ -1504,7 +1504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1569,7 +1569,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1887,8 +1886,8 @@
   <dimension ref="A1:N784"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C379" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A383" sqref="A383"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C76" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="L80" sqref="L80"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -4033,47 +4032,48 @@
       <c r="J80" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K80" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="L80" s="28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="15.75">
+      <c r="K80" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="L80" s="28"/>
+    </row>
+    <row r="81" spans="1:12" ht="15.75">
       <c r="A81" s="17"/>
       <c r="B81" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G81" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J81" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K81" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="L81" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G81" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J81" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="K81" s="58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="15.75">
+    </row>
+    <row r="82" spans="1:12" ht="15.75">
       <c r="A82" s="17"/>
       <c r="B82" s="16" t="s">
         <v>111</v>
@@ -4102,11 +4102,11 @@
       <c r="J82" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K82" s="58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="15.75">
+      <c r="K82" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="15.75">
       <c r="A83" s="17"/>
       <c r="B83" s="16" t="s">
         <v>112</v>
@@ -4135,11 +4135,11 @@
       <c r="J83" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K83" s="58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="15.75">
+      <c r="K83" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="15.75">
       <c r="A84" s="17"/>
       <c r="B84" s="16" t="s">
         <v>113</v>
@@ -4168,16 +4168,16 @@
       <c r="J84" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K84" s="58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="15.75">
+      <c r="K84" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="15.75">
       <c r="A86" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15.75">
+    <row r="87" spans="1:12" ht="15.75">
       <c r="B87" s="16" t="s">
         <v>85</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="15.75">
+    <row r="88" spans="1:12" ht="15.75">
       <c r="B88" s="16" t="s">
         <v>86</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15.75">
+    <row r="89" spans="1:12" ht="15.75">
       <c r="B89" s="16" t="s">
         <v>112</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15.75">
+    <row r="90" spans="1:12" ht="15.75">
       <c r="B90" s="16" t="s">
         <v>116</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="15.75">
+    <row r="91" spans="1:12" ht="15.75">
       <c r="B91" s="16" t="s">
         <v>118</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15.75">
+    <row r="92" spans="1:12" ht="15.75">
       <c r="B92" s="39" t="s">
         <v>119</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15.75">
+    <row r="93" spans="1:12" ht="15.75">
       <c r="B93" s="39" t="s">
         <v>120</v>
       </c>
@@ -4401,12 +4401,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15.75">
+    <row r="95" spans="1:12" ht="15.75">
       <c r="A95" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="15.75">
+    <row r="96" spans="1:12" ht="15.75">
       <c r="B96" s="16" t="s">
         <v>85</v>
       </c>

</xml_diff>